<commit_message>
Added minor error handling to dividendUpdate.py
</commit_message>
<xml_diff>
--- a/dividendCalc.xlsx
+++ b/dividendCalc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FNORD\Desktop\Projects\Finance\dividendTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1D27D2-0A27-4DD4-9CB9-B5A590AD7189}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DF4CFB-A31F-4E02-A903-62706A9C32A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1464" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
     <t>Updated:</t>
   </si>
   <si>
-    <t>2019-07-30 08:00:43.192736</t>
+    <t>2019-07-30 09:22:30.148529</t>
   </si>
   <si>
     <t>OXLC</t>
@@ -69,18 +69,18 @@
     <t>Swing</t>
   </si>
   <si>
+    <t>THW</t>
+  </si>
+  <si>
+    <t>1.40</t>
+  </si>
+  <si>
     <t>NLY</t>
   </si>
   <si>
     <t>1.00</t>
   </si>
   <si>
-    <t>THW</t>
-  </si>
-  <si>
-    <t>1.40</t>
-  </si>
-  <si>
     <t>TCPC</t>
   </si>
   <si>
@@ -102,55 +102,79 @@
     <t>2.44</t>
   </si>
   <si>
+    <t>ABBV</t>
+  </si>
+  <si>
+    <t>4.28</t>
+  </si>
+  <si>
     <t>XOM</t>
   </si>
   <si>
     <t>3.48</t>
   </si>
   <si>
+    <t>PBCT</t>
+  </si>
+  <si>
+    <t>0.71</t>
+  </si>
+  <si>
+    <t>CAH</t>
+  </si>
+  <si>
+    <t>1.92</t>
+  </si>
+  <si>
     <t>LEG</t>
   </si>
   <si>
     <t>1.60</t>
   </si>
   <si>
-    <t>PBCT</t>
-  </si>
-  <si>
-    <t>0.71</t>
-  </si>
-  <si>
-    <t>CAH</t>
-  </si>
-  <si>
-    <t>1.92</t>
-  </si>
-  <si>
     <t>CVX</t>
   </si>
   <si>
     <t>4.76</t>
   </si>
   <si>
+    <t>ADM</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>2.96</t>
+  </si>
+  <si>
+    <t>WBA</t>
+  </si>
+  <si>
+    <t>1.83</t>
+  </si>
+  <si>
     <t>MMM</t>
   </si>
   <si>
     <t>5.76</t>
   </si>
   <si>
-    <t>ADM</t>
-  </si>
-  <si>
-    <t>ED</t>
-  </si>
-  <si>
-    <t>2.96</t>
-  </si>
-  <si>
-    <t>WBA</t>
-  </si>
-  <si>
-    <t>1.83</t>
+    <t>CAT</t>
+  </si>
+  <si>
+    <t>4.12</t>
+  </si>
+  <si>
+    <t>GPC</t>
+  </si>
+  <si>
+    <t>3.05</t>
+  </si>
+  <si>
+    <t>BEN</t>
+  </si>
+  <si>
+    <t>1.04</t>
   </si>
   <si>
     <t>FRT</t>
@@ -159,151 +183,151 @@
     <t>4.08</t>
   </si>
   <si>
-    <t>CAT</t>
-  </si>
-  <si>
-    <t>4.12</t>
+    <t>TGT</t>
+  </si>
+  <si>
+    <t>2.64</t>
   </si>
   <si>
     <t>KO</t>
   </si>
   <si>
+    <t>KMB</t>
+  </si>
+  <si>
     <t>EMR</t>
   </si>
   <si>
     <t>1.96</t>
   </si>
   <si>
-    <t>TGT</t>
-  </si>
-  <si>
-    <t>2.64</t>
-  </si>
-  <si>
-    <t>KMB</t>
-  </si>
-  <si>
-    <t>BEN</t>
-  </si>
-  <si>
-    <t>1.04</t>
-  </si>
-  <si>
     <t>NUE</t>
   </si>
   <si>
-    <t>GPC</t>
-  </si>
-  <si>
-    <t>3.05</t>
-  </si>
-  <si>
     <t>PEP</t>
   </si>
   <si>
     <t>3.82</t>
   </si>
   <si>
+    <t>JNJ</t>
+  </si>
+  <si>
+    <t>3.80</t>
+  </si>
+  <si>
     <t>TROW</t>
   </si>
   <si>
     <t>3.04</t>
   </si>
   <si>
+    <t>ITW</t>
+  </si>
+  <si>
+    <t>4.00</t>
+  </si>
+  <si>
     <t>CLX</t>
   </si>
   <si>
     <t>4.24</t>
   </si>
   <si>
-    <t>ITW</t>
-  </si>
-  <si>
-    <t>4.00</t>
-  </si>
-  <si>
-    <t>JNJ</t>
-  </si>
-  <si>
-    <t>3.80</t>
-  </si>
-  <si>
     <t>PG</t>
   </si>
   <si>
     <t>2.98</t>
   </si>
   <si>
+    <t>SYY</t>
+  </si>
+  <si>
+    <t>1.56</t>
+  </si>
+  <si>
+    <t>UTX</t>
+  </si>
+  <si>
+    <t>2.94</t>
+  </si>
+  <si>
+    <t>GD</t>
+  </si>
+  <si>
+    <t>MCD</t>
+  </si>
+  <si>
+    <t>4.64</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>2.20</t>
+  </si>
+  <si>
+    <t>CINF</t>
+  </si>
+  <si>
+    <t>2.24</t>
+  </si>
+  <si>
+    <t>MDT</t>
+  </si>
+  <si>
+    <t>2.16</t>
+  </si>
+  <si>
+    <t>AOS</t>
+  </si>
+  <si>
+    <t>0.88</t>
+  </si>
+  <si>
+    <t>AFL</t>
+  </si>
+  <si>
+    <t>1.08</t>
+  </si>
+  <si>
+    <t>HRL</t>
+  </si>
+  <si>
+    <t>0.84</t>
+  </si>
+  <si>
+    <t>APD</t>
+  </si>
+  <si>
+    <t>DOV</t>
+  </si>
+  <si>
     <t>VFC</t>
   </si>
   <si>
     <t>1.72</t>
   </si>
   <si>
-    <t>GD</t>
-  </si>
-  <si>
-    <t>UTX</t>
-  </si>
-  <si>
-    <t>2.94</t>
-  </si>
-  <si>
     <t>GWW</t>
   </si>
   <si>
-    <t>MCD</t>
-  </si>
-  <si>
-    <t>4.64</t>
-  </si>
-  <si>
-    <t>SYY</t>
-  </si>
-  <si>
-    <t>1.56</t>
-  </si>
-  <si>
-    <t>MDT</t>
-  </si>
-  <si>
-    <t>2.16</t>
-  </si>
-  <si>
-    <t>CINF</t>
-  </si>
-  <si>
-    <t>2.24</t>
-  </si>
-  <si>
-    <t>LOW</t>
-  </si>
-  <si>
-    <t>2.20</t>
-  </si>
-  <si>
-    <t>APD</t>
-  </si>
-  <si>
-    <t>HRL</t>
-  </si>
-  <si>
-    <t>0.84</t>
-  </si>
-  <si>
     <t>CB</t>
   </si>
   <si>
     <t>3.00</t>
   </si>
   <si>
-    <t>AOS</t>
-  </si>
-  <si>
-    <t>0.88</t>
-  </si>
-  <si>
-    <t>DOV</t>
+    <t>ADP</t>
+  </si>
+  <si>
+    <t>3.16</t>
+  </si>
+  <si>
+    <t>WMT</t>
+  </si>
+  <si>
+    <t>2.12</t>
   </si>
   <si>
     <t>PNR</t>
@@ -312,24 +336,6 @@
     <t>0.72</t>
   </si>
   <si>
-    <t>AFL</t>
-  </si>
-  <si>
-    <t>1.08</t>
-  </si>
-  <si>
-    <t>ADP</t>
-  </si>
-  <si>
-    <t>3.16</t>
-  </si>
-  <si>
-    <t>WMT</t>
-  </si>
-  <si>
-    <t>2.12</t>
-  </si>
-  <si>
     <t>SWK</t>
   </si>
   <si>
@@ -360,25 +366,19 @@
     <t>3.08</t>
   </si>
   <si>
+    <t>SPGI</t>
+  </si>
+  <si>
+    <t>ECL</t>
+  </si>
+  <si>
+    <t>1.84</t>
+  </si>
+  <si>
     <t>SHW</t>
   </si>
   <si>
     <t>4.52</t>
-  </si>
-  <si>
-    <t>SPGI</t>
-  </si>
-  <si>
-    <t>ECL</t>
-  </si>
-  <si>
-    <t>1.84</t>
-  </si>
-  <si>
-    <t>ABBV</t>
-  </si>
-  <si>
-    <t>4.28</t>
   </si>
 </sst>
 </file>
@@ -425,11 +425,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -747,17 +747,17 @@
   <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="8.83984375" style="2" customWidth="1"/>
     <col min="3" max="3" width="8.83984375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.3125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.3125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7890625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.41796875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="1" bestFit="1" customWidth="1"/>
@@ -773,7 +773,7 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -782,10 +782,10 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -794,22 +794,22 @@
         <v>8</v>
       </c>
       <c r="B2" s="2">
-        <v>10.670000076293951</v>
+        <v>10.708000183105471</v>
       </c>
       <c r="C2" s="3">
         <f>D2/B2</f>
-        <v>0.15182755280379345</v>
-      </c>
-      <c r="D2" s="7" t="s">
+        <v>0.15128875348320897</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="2">
         <f>B2/D2</f>
-        <v>6.5864198001814502</v>
+        <v>6.6098766562379447</v>
       </c>
       <c r="F2" s="2">
-        <f>93.720712 * 1.62</f>
-        <v>151.82755344000003</v>
+        <f>93 * 1.62</f>
+        <v>150.66</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
@@ -823,25 +823,25 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2">
-        <v>13.3612003326416</v>
+        <v>13.36359977722168</v>
       </c>
       <c r="C3" s="3">
         <f>D3/B3</f>
-        <v>0.10478100508528267</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>16</v>
+        <v>0.10476219157552942</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E3" s="2">
         <f>B3/D3</f>
-        <v>9.5437145233154297</v>
+        <v>9.5454284123012005</v>
       </c>
       <c r="F3" s="2">
-        <f>74.843575 * 1.4</f>
-        <v>104.78100499999999</v>
+        <f>74 * 1.4</f>
+        <v>103.6</v>
       </c>
       <c r="H3">
         <v>2000</v>
@@ -855,25 +855,25 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2">
-        <v>9.6000003814697266</v>
+        <v>9.619999885559082</v>
       </c>
       <c r="C4" s="3">
         <f>D4/B4</f>
-        <v>0.10416666252745539</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>14</v>
+        <v>0.10395010518670951</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E4" s="2">
         <f>B4/D4</f>
-        <v>9.6000003814697266</v>
+        <v>9.619999885559082</v>
       </c>
       <c r="F4" s="2">
-        <f>104.166663 * 1</f>
-        <v>104.166663</v>
+        <f>103 * 1</f>
+        <v>103</v>
       </c>
       <c r="I4">
         <f>H3*I3</f>
@@ -889,22 +889,22 @@
         <v>17</v>
       </c>
       <c r="B5" s="2">
-        <v>14.060000419616699</v>
+        <v>14.14999961853027</v>
       </c>
       <c r="C5" s="3">
         <f>D5/B5</f>
-        <v>0.1024182046247234</v>
-      </c>
-      <c r="D5" s="7" t="s">
+        <v>0.10176678719582677</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="2">
         <f>B5/D5</f>
-        <v>9.7638891802893752</v>
+        <v>9.826388623979355</v>
       </c>
       <c r="F5" s="2">
-        <f>71.123753 * 1.44</f>
-        <v>102.41820431999999</v>
+        <f>70 * 1.44</f>
+        <v>100.8</v>
       </c>
       <c r="H5" t="s">
         <v>19</v>
@@ -919,22 +919,22 @@
         <v>20</v>
       </c>
       <c r="B6" s="2">
-        <v>31.948099136352539</v>
+        <v>31.954000473022461</v>
       </c>
       <c r="C6" s="3">
         <f>D6/B6</f>
-        <v>8.2947031956109862E-2</v>
-      </c>
-      <c r="D6" s="7" t="s">
+        <v>8.2931713111705482E-2</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="2">
         <f>B6/D6</f>
-        <v>12.055886466548129</v>
+        <v>12.058113386046212</v>
       </c>
       <c r="F6" s="2">
-        <f>31.300767 * 2.65</f>
-        <v>82.947032550000003</v>
+        <f>31 * 2.65</f>
+        <v>82.149999999999991</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -942,68 +942,68 @@
         <v>22</v>
       </c>
       <c r="B7" s="2">
-        <v>29.95999908447266</v>
+        <v>29.97500038146973</v>
       </c>
       <c r="C7" s="3">
         <f>D7/B7</f>
-        <v>8.1441925052146494E-2</v>
-      </c>
-      <c r="D7" s="7" t="s">
+        <v>8.1401166603767103E-2</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="2">
         <f>B7/D7</f>
-        <v>12.278688149374041</v>
+        <v>12.284836221913825</v>
       </c>
       <c r="F7" s="2">
-        <f>33.377838 * 2.44</f>
-        <v>81.441924719999989</v>
+        <f>33 * 2.44</f>
+        <v>80.52</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2">
-        <v>66.860000610351563</v>
-      </c>
-      <c r="C8" s="1">
+        <v>67.150001525878906</v>
+      </c>
+      <c r="C8">
         <f>D8/B8</f>
-        <v>6.4014357776379552E-2</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>116</v>
+        <v>6.3737898775036259E-2</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="E8" s="2">
         <f>B8/D8</f>
-        <v>15.621495469708307</v>
+        <v>15.689252692962361</v>
       </c>
       <c r="F8" s="2">
-        <f>14.956626 * 4.28</f>
-        <v>64.014359280000008</v>
+        <f>14 * 4.28</f>
+        <v>59.92</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" s="2">
-        <v>75.3865966796875</v>
+        <v>74.985000610351563</v>
       </c>
       <c r="C9" s="3">
         <f>D9/B9</f>
-        <v>4.6162052052651774E-2</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>25</v>
+        <v>4.6409281478616025E-2</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="E9" s="2">
         <f>B9/D9</f>
-        <v>21.662815137841235</v>
+        <v>21.547413968491828</v>
       </c>
       <c r="F9" s="2">
-        <f>13.264957 * 3.48</f>
-        <v>46.162050360000002</v>
+        <f>13 * 3.48</f>
+        <v>45.24</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1011,22 +1011,22 @@
         <v>28</v>
       </c>
       <c r="B10" s="2">
-        <v>16.469999313354489</v>
+        <v>16.530000686645511</v>
       </c>
       <c r="C10" s="3">
         <f>D10/B10</f>
-        <v>4.3108684250175139E-2</v>
-      </c>
-      <c r="D10" s="7" t="s">
+        <v>4.29522063222662E-2</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>29</v>
       </c>
       <c r="E10" s="2">
         <f>B10/D10</f>
-        <v>23.197182131485196</v>
+        <v>23.281691107951424</v>
       </c>
       <c r="F10" s="2">
-        <f>60.716457 * 0.71</f>
-        <v>43.10868447</v>
+        <f>60 * 0.71</f>
+        <v>42.599999999999994</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1034,68 +1034,68 @@
         <v>30</v>
       </c>
       <c r="B11" s="2">
-        <v>45.650001525878913</v>
+        <v>46.159999847412109</v>
       </c>
       <c r="C11" s="3">
         <f>D11/B11</f>
-        <v>4.205914426775112E-2</v>
-      </c>
-      <c r="D11" s="7" t="s">
+        <v>4.159445421028618E-2</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E11" s="2">
         <f>B11/D11</f>
-        <v>23.776042461395267</v>
+        <v>24.041666587193809</v>
       </c>
       <c r="F11" s="2">
-        <f>21.905804 * 1.92</f>
-        <v>42.059143679999998</v>
+        <f>21 * 1.92</f>
+        <v>40.32</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B12" s="2">
-        <v>39.75</v>
+        <v>40.779998779296882</v>
       </c>
       <c r="C12" s="3">
         <f>D12/B12</f>
-        <v>4.025157232704403E-2</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>27</v>
+        <v>3.9234920252432311E-2</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="E12" s="2">
         <f>B12/D12</f>
-        <v>24.84375</v>
+        <v>25.48749923706055</v>
       </c>
       <c r="F12" s="2">
-        <f>25.157233 * 1.6</f>
-        <v>40.251572800000005</v>
+        <f>24 * 1.6</f>
+        <v>38.400000000000006</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2">
-        <v>124.5350036621094</v>
+        <v>123.5699996948242</v>
       </c>
       <c r="C13" s="3">
         <f>D13/B13</f>
-        <v>3.8222185409934356E-2</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>33</v>
+        <v>3.852067663474612E-2</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="E13" s="2">
         <f>B13/D13</f>
-        <v>26.162815895401135</v>
+        <v>25.960083969500886</v>
       </c>
       <c r="F13" s="2">
-        <f>8.029871 * 4.76</f>
-        <v>38.222185959999997</v>
+        <f>8 * 4.76</f>
+        <v>38.08</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1103,827 +1103,827 @@
         <v>36</v>
       </c>
       <c r="B14" s="2">
-        <v>40.599998474121087</v>
+        <v>40.919998168945313</v>
       </c>
       <c r="C14" s="3">
         <f>D14/B14</f>
-        <v>3.4482759916662963E-2</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>16</v>
+        <v>3.4213100260167585E-2</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="E14" s="2">
         <f>B14/D14</f>
-        <v>28.999998910086493</v>
+        <v>29.228570120675226</v>
       </c>
       <c r="F14" s="2">
-        <f>24.630543 * 1.4</f>
-        <v>34.482760199999994</v>
+        <f>24 * 1.4</f>
+        <v>33.599999999999994</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B15" s="2">
-        <v>86.580001831054688</v>
+        <v>55.119998931884773</v>
       </c>
       <c r="C15" s="3">
         <f>D15/B15</f>
-        <v>3.4188033465001627E-2</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>38</v>
+        <v>3.320029091911713E-2</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="E15" s="2">
         <f>B15/D15</f>
-        <v>29.250000618599557</v>
+        <v>30.120217995565447</v>
       </c>
       <c r="F15" s="2">
-        <f>11.550011 * 2.96</f>
-        <v>34.188032559999996</v>
+        <f>18 * 1.83</f>
+        <v>32.94</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" s="2">
-        <v>54.744998931884773</v>
+        <v>86.069999694824219</v>
       </c>
       <c r="C16" s="3">
         <f>D16/B16</f>
-        <v>3.3427710945376693E-2</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>40</v>
+        <v>3.4390612414257955E-2</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="E16" s="2">
         <f>B16/D16</f>
-        <v>29.915299962778562</v>
+        <v>29.077702599602777</v>
       </c>
       <c r="F16" s="2">
-        <f>18.266509 * 1.83</f>
-        <v>33.427711469999998</v>
+        <f>11 * 2.96</f>
+        <v>32.56</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B17" s="2">
-        <v>175.19000244140619</v>
+        <v>98.091499328613281</v>
       </c>
       <c r="C17" s="3">
         <f>D17/B17</f>
-        <v>3.2878588502368918E-2</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>35</v>
+        <v>3.109341809306319E-2</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E17" s="2">
         <f>B17/D17</f>
-        <v>30.414930979410798</v>
+        <v>32.161147320856813</v>
       </c>
       <c r="F17" s="2">
-        <f>5.708088 * 5.76</f>
-        <v>32.87858688</v>
+        <f>10 * 3.05</f>
+        <v>30.5</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B18" s="2">
-        <v>132.36000061035159</v>
+        <v>33.569999694824219</v>
       </c>
       <c r="C18" s="3">
         <f>D18/B18</f>
-        <v>3.1127228626484184E-2</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>44</v>
+        <v>3.0980041985533471E-2</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="E18" s="2">
         <f>B18/D18</f>
-        <v>32.126213740376599</v>
+        <v>32.278845860407898</v>
       </c>
       <c r="F18" s="2">
-        <f>7.555153 * 4.12</f>
-        <v>31.127230359999999</v>
+        <f>29 * 1.04</f>
+        <v>30.16</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B19" s="2">
-        <v>98.239997863769531</v>
+        <v>86.470001220703125</v>
       </c>
       <c r="C19" s="3">
         <f>D19/B19</f>
-        <v>3.1046417613215627E-2</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>55</v>
+        <v>3.0530819506544852E-2</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="E19" s="2">
         <f>B19/D19</f>
-        <v>32.209835365170342</v>
+        <v>32.753788341175422</v>
       </c>
       <c r="F19" s="2">
-        <f>10.179153 * 3.05</f>
-        <v>31.046416649999998</v>
+        <f>11 * 2.64</f>
+        <v>29.040000000000003</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B20" s="2">
-        <v>33.590000152587891</v>
+        <v>133.20649719238281</v>
       </c>
       <c r="C20" s="3">
         <f>D20/B20</f>
-        <v>3.0961595572361878E-2</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>52</v>
+        <v>3.0929422264213666E-2</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="E20" s="2">
         <f>B20/D20</f>
-        <v>32.298077069796051</v>
+        <v>32.33167407582107</v>
       </c>
       <c r="F20" s="2">
-        <f>29.770765 * 1.04</f>
-        <v>30.961595600000003</v>
+        <f>7 * 4.12</f>
+        <v>28.84</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B21" s="2">
-        <v>132.5</v>
+        <v>138.6499938964844</v>
       </c>
       <c r="C21" s="3">
         <f>D21/B21</f>
-        <v>3.079245283018868E-2</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>42</v>
+        <v>2.9715111297271155E-2</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="E21" s="2">
         <f>B21/D21</f>
-        <v>32.475490196078432</v>
+        <v>33.652911139923397</v>
       </c>
       <c r="F21" s="2">
-        <f>7.54717 * 4.08</f>
-        <v>30.792453600000002</v>
+        <f>7 * 4.12</f>
+        <v>28.84</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B22" s="2">
-        <v>86.599998474121094</v>
+        <v>54.139999389648438</v>
       </c>
       <c r="C22" s="3">
         <f>D22/B22</f>
-        <v>3.0484988989796787E-2</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>49</v>
+        <v>2.9553011046134586E-2</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="E22" s="2">
         <f>B22/D22</f>
-        <v>32.803029725045867</v>
+        <v>33.837499618530273</v>
       </c>
       <c r="F22" s="2">
-        <f>11.547344 * 2.64</f>
-        <v>30.484988160000004</v>
+        <f>18 * 1.6</f>
+        <v>28.8</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B23" s="2">
-        <v>54.200000762939453</v>
+        <v>176.42999267578119</v>
       </c>
       <c r="C23" s="3">
         <f>D23/B23</f>
-        <v>2.9520294787413331E-2</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>27</v>
+        <v>3.2647510282364157E-2</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="E23" s="2">
         <f>B23/D23</f>
-        <v>33.875000476837158</v>
+        <v>30.630207061767571</v>
       </c>
       <c r="F23" s="2">
-        <f>18.450184 * 1.6</f>
-        <v>29.520294400000001</v>
+        <f>5 * 5.76</f>
+        <v>28.799999999999997</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" s="2">
-        <v>139.61000061035159</v>
+        <v>131.8800048828125</v>
       </c>
       <c r="C24" s="3">
         <f>D24/B24</f>
-        <v>2.9510779901067607E-2</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>44</v>
+        <v>3.0937214505151519E-2</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="E24" s="2">
         <f>B24/D24</f>
-        <v>33.88592247824068</v>
+        <v>32.323530608532472</v>
       </c>
       <c r="F24" s="2">
-        <f>7.162811 * 4.12</f>
-        <v>29.51078132</v>
+        <f>7 * 4.08</f>
+        <v>28.560000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B25" s="2">
-        <v>66.658599853515625</v>
+        <v>66.769996643066406</v>
       </c>
       <c r="C25" s="3">
         <f>D25/B25</f>
-        <v>2.9403557895112734E-2</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>47</v>
+        <v>2.9354502000016682E-2</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="E25" s="2">
         <f>B25/D25</f>
-        <v>34.009489721181438</v>
+        <v>34.066324817891022</v>
       </c>
       <c r="F25" s="2">
-        <f>15.001815 * 1.96</f>
-        <v>29.4035574</v>
+        <f>14 * 1.96</f>
+        <v>27.439999999999998</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B26" s="2">
-        <v>55.229999542236328</v>
+        <v>55.595901489257813</v>
       </c>
       <c r="C26" s="3">
         <f>D26/B26</f>
-        <v>2.8969763050177535E-2</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>27</v>
+        <v>2.877909984622069E-2</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="E26" s="2">
         <f>B26/D26</f>
-        <v>34.518749713897705</v>
+        <v>34.747438430786133</v>
       </c>
       <c r="F26" s="2">
-        <f>18.106102 * 1.6</f>
-        <v>28.969763200000003</v>
+        <f>17 * 1.6</f>
+        <v>27.200000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B27" s="2">
-        <v>131.88240051269531</v>
+        <v>131.3500061035156</v>
       </c>
       <c r="C27" s="3">
         <f>D27/B27</f>
-        <v>2.8965199186166447E-2</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>57</v>
+        <v>2.9082602379093131E-2</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="E27" s="2">
         <f>B27/D27</f>
-        <v>34.524188615888825</v>
+        <v>34.384818351705654</v>
       </c>
       <c r="F27" s="2">
-        <f>7.582513 * 3.82</f>
-        <v>28.965199659999996</v>
+        <f>7 * 3.82</f>
+        <v>26.74</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B28" s="2">
-        <v>131.55000305175781</v>
+        <v>132.1217041015625</v>
       </c>
       <c r="C28" s="3">
         <f>D28/B28</f>
-        <v>2.8886354327980559E-2</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>65</v>
+        <v>2.8761360791100032E-2</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="E28" s="2">
         <f>B28/D28</f>
-        <v>34.618421855725742</v>
+        <v>34.768869500411185</v>
       </c>
       <c r="F28" s="2">
-        <f>7.601672 * 3.8</f>
-        <v>28.886353599999996</v>
+        <f>7 * 3.8</f>
+        <v>26.599999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B29" s="2">
-        <v>113.86000061035161</v>
+        <v>153.4700012207031</v>
       </c>
       <c r="C29" s="3">
         <f>D29/B29</f>
-        <v>2.6699455328508207E-2</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>59</v>
+        <v>2.6063725602293149E-2</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="E29" s="2">
         <f>B29/D29</f>
-        <v>37.453947569194604</v>
+        <v>38.367500305175774</v>
       </c>
       <c r="F29" s="2">
-        <f>8.782716 * 3.04</f>
-        <v>26.699456640000001</v>
+        <f>6.515931 * 4</f>
+        <v>26.063724000000001</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B30" s="2">
-        <v>153.4700012207031</v>
+        <v>165.1300048828125</v>
       </c>
       <c r="C30" s="3">
         <f>D30/B30</f>
-        <v>2.6063725602293149E-2</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>63</v>
+        <v>2.5676738779296913E-2</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="E30" s="2">
         <f>B30/D30</f>
-        <v>38.367500305175774</v>
+        <v>38.945755868587852</v>
       </c>
       <c r="F30" s="2">
-        <f>6.515931 * 4</f>
-        <v>26.063724000000001</v>
+        <f>6 * 4.24</f>
+        <v>25.44</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B31" s="2">
-        <v>165.74000549316409</v>
+        <v>165.1300048828125</v>
       </c>
       <c r="C31" s="3">
         <f>D31/B31</f>
-        <v>2.5582236391170375E-2</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>61</v>
+        <v>2.5676738779296913E-2</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="E31" s="2">
         <f>B31/D31</f>
-        <v>39.089623937067003</v>
+        <v>38.945755868587852</v>
       </c>
       <c r="F31" s="2">
-        <f>6.033546 * 4.24</f>
-        <v>25.582235040000004</v>
+        <f>6 * 4.24</f>
+        <v>25.44</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B32" s="2">
-        <v>165.77000427246091</v>
+        <v>114.0699996948242</v>
       </c>
       <c r="C32" s="3">
         <f>D32/B32</f>
-        <v>2.5577606869280779E-2</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>61</v>
+        <v>2.6650302517165138E-2</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="E32" s="2">
         <f>B32/D32</f>
-        <v>39.09669912086342</v>
+        <v>37.523026215402702</v>
       </c>
       <c r="F32" s="2">
-        <f>6.032454 * 4.24</f>
-        <v>25.577604960000002</v>
+        <f>8 * 3.04</f>
+        <v>24.32</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B33" s="2">
-        <v>120.76499938964839</v>
+        <v>120.90000152587891</v>
       </c>
       <c r="C33" s="3">
         <f>D33/B33</f>
-        <v>2.4676023807072005E-2</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>67</v>
+        <v>2.4648469498671798E-2</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="E33" s="2">
         <f>B33/D33</f>
-        <v>40.525167580418923</v>
+        <v>40.570470310697623</v>
       </c>
       <c r="F33" s="2">
-        <f>8.280545 * 2.98</f>
-        <v>24.676024099999999</v>
+        <f>8 * 2.98</f>
+        <v>23.84</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B34" s="2">
-        <v>69.785003662109375</v>
+        <v>69.635002136230469</v>
       </c>
       <c r="C34" s="3">
         <f>D34/B34</f>
-        <v>2.2354372976081411E-2</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>77</v>
+        <v>2.2402526777382636E-2</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="E34" s="2">
         <f>B34/D34</f>
-        <v>44.73397670648037</v>
+        <v>44.63782188219902</v>
       </c>
       <c r="F34" s="2">
-        <f>14.329726 * 1.56</f>
-        <v>22.354372560000002</v>
+        <f>14 * 1.56</f>
+        <v>21.84</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B35" s="2">
-        <v>134.9100036621094</v>
+        <v>135.4400939941406</v>
       </c>
       <c r="C35" s="3">
         <f>D35/B35</f>
-        <v>2.1792305390217134E-2</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>72</v>
+        <v>2.170701387823306E-2</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="E35" s="2">
         <f>B35/D35</f>
-        <v>45.887756347656257</v>
+        <v>46.068059181680475</v>
       </c>
       <c r="F35" s="2">
-        <f>7.412349 * 2.94</f>
-        <v>21.792306059999998</v>
+        <f>7 * 2.94</f>
+        <v>20.58</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B36" s="2">
-        <v>188.86000061035159</v>
+        <v>189.1000061035156</v>
       </c>
       <c r="C36" s="3">
         <f>D36/B36</f>
-        <v>2.1603303964917872E-2</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>42</v>
+        <v>2.1575885078324954E-2</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="E36" s="2">
         <f>B36/D36</f>
-        <v>46.289215835870486</v>
+        <v>46.348040711645979</v>
       </c>
       <c r="F36" s="2">
-        <f>5.294927 * 4.08</f>
-        <v>21.603302160000002</v>
+        <f>5 * 4.08</f>
+        <v>20.399999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B37" s="2">
-        <v>215.1300048828125</v>
+        <v>106.0800018310547</v>
       </c>
       <c r="C37" s="3">
         <f>D37/B37</f>
-        <v>2.156835352896283E-2</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>75</v>
+        <v>2.1116138398710366E-2</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="E37" s="2">
         <f>B37/D37</f>
-        <v>46.364225190261315</v>
+        <v>47.357143674577991</v>
       </c>
       <c r="F37" s="2">
-        <f>4.648352 * 4.64</f>
-        <v>21.56835328</v>
+        <f>9 * 2.24</f>
+        <v>20.160000000000004</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B38" s="2">
-        <v>103.1699981689453</v>
+        <v>103.9100036621094</v>
       </c>
       <c r="C38" s="3">
         <f>D38/B38</f>
-        <v>2.1324028681258728E-2</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>83</v>
+        <v>2.1172167476327653E-2</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="E38" s="2">
         <f>B38/D38</f>
-        <v>46.895453713156947</v>
+        <v>47.231819846413359</v>
       </c>
       <c r="F38" s="2">
-        <f>9.69274 * 2.2</f>
-        <v>21.324028000000002</v>
+        <f>9 * 2.2</f>
+        <v>19.8</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B39" s="2">
-        <v>106.4199981689453</v>
+        <v>103.6600036621094</v>
       </c>
       <c r="C39" s="3">
         <f>D39/B39</f>
-        <v>2.1048675423240709E-2</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>81</v>
+        <v>2.0837352148286099E-2</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="E39" s="2">
         <f>B39/D39</f>
-        <v>47.508927753993433</v>
+        <v>47.99074243616176</v>
       </c>
       <c r="F39" s="2">
-        <f>9.39673 * 2.24</f>
-        <v>21.048675200000002</v>
+        <f>9 * 2.16</f>
+        <v>19.440000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B40" s="2">
-        <v>103.4700012207031</v>
+        <v>53.069999694824219</v>
       </c>
       <c r="C40" s="3">
         <f>D40/B40</f>
-        <v>2.0875615874331413E-2</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>79</v>
+        <v>2.0350480614480384E-2</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="E40" s="2">
         <f>B40/D40</f>
-        <v>47.902778342918097</v>
+        <v>49.138888606318716</v>
       </c>
       <c r="F40" s="2">
-        <f>9.664637 * 2.16</f>
-        <v>20.875615920000005</v>
+        <f>18 * 1.08</f>
+        <v>19.440000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B41" s="2">
-        <v>42.580001831054688</v>
+        <v>44.909999847412109</v>
       </c>
       <c r="C41" s="3">
         <f>D41/B41</f>
-        <v>2.0666978913988526E-2</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>90</v>
+        <v>1.9594745112222686E-2</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="E41" s="2">
         <f>B41/D41</f>
-        <v>48.386365717107601</v>
+        <v>51.034090735695578</v>
       </c>
       <c r="F41" s="2">
-        <f>23.485203 * 0.88</f>
-        <v>20.66697864</v>
+        <f>22 * 0.88</f>
+        <v>19.36</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B42" s="2">
-        <v>53.074199676513672</v>
+        <v>41.689998626708977</v>
       </c>
       <c r="C42" s="3">
         <f>D42/B42</f>
-        <v>2.03488701964906E-2</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>95</v>
+        <v>2.014871738234715E-2</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="E42" s="2">
         <f>B42/D42</f>
-        <v>49.1427774782534</v>
+        <v>49.630950746082121</v>
       </c>
       <c r="F42" s="2">
-        <f>18.841546 * 1.08</f>
-        <v>20.348869680000004</v>
+        <f>23 * 0.84</f>
+        <v>19.32</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B43" s="2">
-        <v>41.619998931884773</v>
+        <v>96.930000305175781</v>
       </c>
       <c r="C43" s="3">
         <f>D43/B43</f>
-        <v>2.0182605035015563E-2</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>86</v>
+        <v>1.9808108882235064E-2</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="E43" s="2">
         <f>B43/D43</f>
-        <v>49.547617776053301</v>
+        <v>50.484375158945724</v>
       </c>
       <c r="F43" s="2">
-        <f>24.026911 * 0.84</f>
-        <v>20.182605239999997</v>
+        <f>10 * 1.92</f>
+        <v>19.2</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B44" s="2">
-        <v>231.2850036621094</v>
+        <v>88.468696594238281</v>
       </c>
       <c r="C44" s="3">
         <f>D44/B44</f>
-        <v>2.0061828162359817E-2</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>75</v>
+        <v>1.9441905060371589E-2</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="E44" s="2">
         <f>B44/D44</f>
-        <v>49.845905961661515</v>
+        <v>51.435288717580399</v>
       </c>
       <c r="F44" s="2">
-        <f>4.32367 * 4.64</f>
-        <v>20.061828799999997</v>
+        <f>11 * 1.72</f>
+        <v>18.919999999999998</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B45" s="2">
-        <v>96.708099365234375</v>
+        <v>213.91999816894531</v>
       </c>
       <c r="C45" s="3">
         <f>D45/B45</f>
-        <v>1.985355944954308E-2</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>31</v>
+        <v>2.1690351718942687E-2</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="E45" s="2">
         <f>B45/D45</f>
-        <v>50.368801752726242</v>
+        <v>46.103447881238218</v>
       </c>
       <c r="F45" s="2">
-        <f>10.340396 * 1.92</f>
-        <v>19.85356032</v>
+        <f>4 * 4.64</f>
+        <v>18.559999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="B46" s="2">
-        <v>87.430000305175781</v>
+        <v>231.9700012207031</v>
       </c>
       <c r="C46" s="3">
         <f>D46/B46</f>
-        <v>1.9672881093404017E-2</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>69</v>
+        <v>2.0002586436102861E-2</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="E46" s="2">
         <f>B46/D46</f>
-        <v>50.831395526264991</v>
+        <v>49.993534745841188</v>
       </c>
       <c r="F46" s="2">
-        <f>11.437722 * 1.72</f>
-        <v>19.672881840000002</v>
+        <f>4 * 4.64</f>
+        <v>18.559999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="B47" s="2">
-        <v>293.76998901367188</v>
+        <v>153.1499938964844</v>
       </c>
       <c r="C47" s="3">
         <f>D47/B47</f>
-        <v>1.9607176414919405E-2</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>35</v>
+        <v>1.9588639370287729E-2</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="E47" s="2">
         <f>B47/D47</f>
-        <v>51.001734203762481</v>
+        <v>51.049997965494804</v>
       </c>
       <c r="F47" s="2">
-        <f>3.404024 * 5.76</f>
-        <v>19.60717824</v>
+        <f>6 * 3</f>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="B48" s="2">
-        <v>153.6300048828125</v>
+        <v>38.919998168945313</v>
       </c>
       <c r="C48" s="3">
         <f>D48/B48</f>
-        <v>1.952743542700771E-2</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>88</v>
+        <v>1.8499486995723853E-2</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="E48" s="2">
         <f>B48/D48</f>
-        <v>51.210001627604164</v>
+        <v>54.055553012424049</v>
       </c>
       <c r="F48" s="2">
-        <f>6.509145 * 3</f>
-        <v>19.527435000000001</v>
+        <f>25 * 0.72</f>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B49" s="2">
-        <v>167.32499694824219</v>
+        <v>295.677001953125</v>
       </c>
       <c r="C49" s="3">
         <f>D49/B49</f>
-        <v>1.8885403003936509E-2</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>97</v>
+        <v>1.9480717005217599E-2</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="E49" s="2">
         <f>B49/D49</f>
-        <v>52.950948401342465</v>
+        <v>51.332812839084205</v>
       </c>
       <c r="F49" s="2">
-        <f>5.976393 * 3.16</f>
-        <v>18.88540188</v>
+        <f>3 * 5.76</f>
+        <v>17.28</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1931,160 +1931,160 @@
         <v>98</v>
       </c>
       <c r="B50" s="2">
-        <v>112.26280212402339</v>
+        <v>112.245002746582</v>
       </c>
       <c r="C50" s="3">
         <f>D50/B50</f>
-        <v>1.8884260502048666E-2</v>
-      </c>
-      <c r="D50" s="7" t="s">
+        <v>1.8887255094878215E-2</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>99</v>
       </c>
       <c r="E50" s="2">
         <f>B50/D50</f>
-        <v>52.954151945294051</v>
+        <v>52.945756012538681</v>
       </c>
       <c r="F50" s="2">
-        <f>8.90767 * 2.12</f>
-        <v>18.884260399999999</v>
+        <f>8 * 2.12</f>
+        <v>16.96</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B51" s="2">
-        <v>38.70989990234375</v>
+        <v>151.0350036621094</v>
       </c>
       <c r="C51" s="3">
         <f>D51/B51</f>
-        <v>1.8599893097538248E-2</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>93</v>
+        <v>1.8273909577772991E-2</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="E51" s="2">
         <f>B51/D51</f>
-        <v>53.763749864366325</v>
+        <v>54.722827413807757</v>
       </c>
       <c r="F51" s="2">
-        <f>25.833185 * 0.72</f>
-        <v>18.5998932</v>
+        <f>6 * 2.76</f>
+        <v>16.559999999999999</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B52" s="2">
-        <v>149.13999938964841</v>
+        <v>119.120002746582</v>
       </c>
       <c r="C52" s="3">
         <f>D52/B52</f>
-        <v>1.8506101725192629E-2</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>101</v>
+        <v>1.7125587247843941E-2</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="E52" s="2">
         <f>B52/D52</f>
-        <v>54.036231662916094</v>
+        <v>58.392158209108821</v>
       </c>
       <c r="F52" s="2">
-        <f>6.705109 * 2.76</f>
-        <v>18.506100839999998</v>
+        <f>8 * 2.04</f>
+        <v>16.32</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B53" s="2">
-        <v>118.30999755859381</v>
+        <v>167.11000061035159</v>
       </c>
       <c r="C53" s="3">
         <f>D53/B53</f>
-        <v>1.72428369714882E-2</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>103</v>
+        <v>1.8909700128409038E-2</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="E53" s="2">
         <f>B53/D53</f>
-        <v>57.995096842447943</v>
+        <v>52.882911585554297</v>
       </c>
       <c r="F53" s="2">
-        <f>8.452371 * 2.04</f>
-        <v>17.242836839999999</v>
+        <f>5 * 3.16</f>
+        <v>15.8</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B54" s="2">
-        <v>88.370002746582031</v>
+        <v>88.484703063964844</v>
       </c>
       <c r="C54" s="3">
         <f>D54/B54</f>
-        <v>1.4484553131345328E-2</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>105</v>
+        <v>1.4465777198514175E-2</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>107</v>
       </c>
       <c r="E54" s="2">
         <f>B54/D54</f>
-        <v>69.039064645767212</v>
+        <v>69.128674268722534</v>
       </c>
       <c r="F54" s="2">
-        <f>11.316057 * 1.28</f>
-        <v>14.484552960000002</v>
+        <f>11 * 1.28</f>
+        <v>14.08</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B55" s="2">
-        <v>163.3699951171875</v>
+        <v>163.18499755859381</v>
       </c>
       <c r="C55" s="3">
         <f>D55/B55</f>
-        <v>1.395605109961915E-2</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>107</v>
+        <v>1.3971872623776794E-2</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="E55" s="2">
         <f>B55/D55</f>
-        <v>71.653506630345404</v>
+        <v>71.57236735026045</v>
       </c>
       <c r="F55" s="2">
-        <f>6.121075 * 2.28</f>
-        <v>13.956050999999999</v>
+        <f>6 * 2.28</f>
+        <v>13.68</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B56" s="2">
-        <v>255.6000061035156</v>
+        <v>256.73001098632813</v>
       </c>
       <c r="C56" s="3">
         <f>D56/B56</f>
-        <v>1.2050077959515498E-2</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>109</v>
+        <v>1.1997039178111599E-2</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="E56" s="2">
         <f>B56/D56</f>
-        <v>82.98701496867389</v>
+        <v>83.353899670885752</v>
       </c>
       <c r="F56" s="2">
-        <f>3.912363 * 3.08</f>
-        <v>12.050078040000001</v>
+        <f>3 * 3.08</f>
+        <v>9.24</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2092,68 +2092,68 @@
         <v>112</v>
       </c>
       <c r="B57" s="2">
-        <v>242.02000427246091</v>
+        <v>241.97999572753909</v>
       </c>
       <c r="C57" s="3">
         <f>D57/B57</f>
-        <v>9.4207088660044191E-3</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>107</v>
+        <v>9.4222664693621987E-3</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="E57" s="2">
         <f>B57/D57</f>
-        <v>106.14912468090391</v>
+        <v>106.13157707348206</v>
       </c>
       <c r="F57" s="2">
-        <f>4.13189 * 2.28</f>
-        <v>9.4207091999999992</v>
+        <f>4 * 2.28</f>
+        <v>9.1199999999999992</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B58" s="2">
-        <v>207.75999450683591</v>
+        <v>510.42001342773438</v>
       </c>
       <c r="C58" s="3">
         <f>D58/B58</f>
-        <v>8.856372971936418E-3</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>114</v>
+        <v>8.8554521395935518E-3</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="E58" s="2">
         <f>B58/D58</f>
-        <v>112.9130404928456</v>
+        <v>112.92478173179965</v>
       </c>
       <c r="F58" s="2">
-        <f>4.813246 * 1.84</f>
-        <v>8.8563726400000018</v>
+        <f>1.959171 * 4.52</f>
+        <v>8.8554529199999994</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B59" s="2">
-        <v>510.42001342773438</v>
+        <v>206.92999267578119</v>
       </c>
       <c r="C59" s="3">
         <f>D59/B59</f>
-        <v>8.8554521395935518E-3</v>
-      </c>
-      <c r="D59" s="7" t="s">
-        <v>111</v>
+        <v>8.8918961249030738E-3</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="E59" s="2">
         <f>B59/D59</f>
-        <v>112.92478173179965</v>
+        <v>112.46195254118543</v>
       </c>
       <c r="F59" s="2">
-        <f>1.959171 * 4.52</f>
-        <v>8.8554529199999994</v>
+        <f>4 * 1.84</f>
+        <v>7.36</v>
       </c>
     </row>
   </sheetData>
@@ -2161,6 +2161,6 @@
     <sortCondition descending="1" ref="F2:F59"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated spreadsheet to new format and added handling of different yield styles
</commit_message>
<xml_diff>
--- a/dividendCalc.xlsx
+++ b/dividendCalc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FNORD\Desktop\Projects\Finance\dividendTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2184FF94-EB53-4138-84B2-B10BDAECAA25}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CD774C-7D3B-409E-AE4B-DC3F4223EDAF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10296" yWindow="312" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="120">
   <si>
     <t>Stock ID</t>
   </si>
@@ -39,13 +39,7 @@
     <t>Yield</t>
   </si>
   <si>
-    <t>Recurrence</t>
-  </si>
-  <si>
     <t>Annual Yield</t>
-  </si>
-  <si>
-    <t>$stock/$div</t>
   </si>
   <si>
     <t>$price/annual yield</t>
@@ -759,29 +753,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M62"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L16" sqref="L16"/>
+      <selection pane="bottomRight" activeCell="A63" sqref="A63:D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="8.83984375" style="3" customWidth="1"/>
     <col min="3" max="3" width="8.83984375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.62890625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83984375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="10.3125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7890625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.83984375" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.47265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7890625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.83984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -791,2140 +782,1470 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="6" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
         <v>8</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>10</v>
       </c>
       <c r="B2" s="3">
         <v>10.760000228881839</v>
       </c>
       <c r="C2" s="4">
-        <f t="shared" ref="C2:C33" si="0">F2/B2</f>
+        <f>D2/B2</f>
         <v>0.15055761761525052</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6">
+        <f>B2/D2</f>
+        <v>6.6419754499270613</v>
+      </c>
+      <c r="F2" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B2)*D2</f>
+        <v>149.04000000000002</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="6">
-        <f t="shared" ref="E2:E33" si="1">F2/D2</f>
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="6">
-        <f t="shared" ref="G2:G33" si="2">B2/E2</f>
-        <v>79.703705399124729</v>
-      </c>
-      <c r="H2" s="6">
-        <f t="shared" ref="H2:H33" si="3">B2/F2</f>
-        <v>6.6419754499270613</v>
-      </c>
-      <c r="I2" s="7">
-        <f t="shared" ref="I2:I33" si="4">_xlfn.FLOOR.MATH(1000/B2)*F2</f>
-        <v>149.04000000000002</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
         <v>13</v>
-      </c>
-      <c r="M2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>15</v>
       </c>
       <c r="B3" s="3">
         <v>9.3500003814697266</v>
       </c>
       <c r="C3" s="4">
-        <f t="shared" si="0"/>
+        <f>D3/B3</f>
         <v>0.10695186729423534</v>
       </c>
-      <c r="D3">
-        <v>4</v>
+      <c r="D3" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E3" s="6">
-        <f t="shared" si="1"/>
+        <f>B3/D3</f>
+        <v>9.3500003814697266</v>
+      </c>
+      <c r="F3" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B3)*D3</f>
+        <v>106</v>
+      </c>
+      <c r="H3">
+        <v>2000</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="J3" s="5">
         <v>0.25</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="6">
-        <f t="shared" si="2"/>
-        <v>37.400001525878906</v>
-      </c>
-      <c r="H3" s="6">
-        <f t="shared" si="3"/>
-        <v>9.3500003814697266</v>
-      </c>
-      <c r="I3" s="7">
-        <f t="shared" si="4"/>
-        <v>106</v>
-      </c>
-      <c r="K3">
-        <v>2000</v>
-      </c>
-      <c r="L3" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="M3" s="5">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3">
         <v>13.33250045776367</v>
       </c>
       <c r="C4" s="4">
-        <f t="shared" si="0"/>
+        <f>D4/B4</f>
         <v>0.10500655930484244</v>
       </c>
-      <c r="D4">
-        <v>12</v>
+      <c r="D4" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="E4" s="6">
-        <f t="shared" si="1"/>
-        <v>0.11666666666666665</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="6">
-        <f t="shared" si="2"/>
-        <v>114.27857535226003</v>
-      </c>
-      <c r="H4" s="6">
-        <f t="shared" si="3"/>
+        <f>B4/D4</f>
         <v>9.5232146126883368</v>
       </c>
-      <c r="I4" s="7">
-        <f t="shared" si="4"/>
+      <c r="F4" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B4)*D4</f>
         <v>105</v>
       </c>
-      <c r="L4">
-        <f>K3*L3</f>
+      <c r="I4">
+        <f>H3*I3</f>
         <v>1500</v>
       </c>
-      <c r="M4">
-        <f>K3*M3</f>
+      <c r="J4">
+        <f>H3*J3</f>
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3">
         <v>14.10000038146973</v>
       </c>
       <c r="C5" s="4">
-        <f t="shared" si="0"/>
+        <f>D5/B5</f>
         <v>0.10212765681144612</v>
       </c>
-      <c r="D5">
-        <v>4</v>
+      <c r="D5" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="E5" s="6">
-        <f t="shared" si="1"/>
-        <v>0.36</v>
-      </c>
-      <c r="F5" s="6" t="s">
+        <f>B5/D5</f>
+        <v>9.7916669315762022</v>
+      </c>
+      <c r="F5" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B5)*D5</f>
+        <v>100.8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5">
+        <f>I4*0.25</f>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
         <v>20</v>
-      </c>
-      <c r="G5" s="6">
-        <f t="shared" si="2"/>
-        <v>39.166667726304809</v>
-      </c>
-      <c r="H5" s="6">
-        <f t="shared" si="3"/>
-        <v>9.7916669315762022</v>
-      </c>
-      <c r="I5" s="7">
-        <f t="shared" si="4"/>
-        <v>100.8</v>
-      </c>
-      <c r="K5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5">
-        <f>L4*0.25</f>
-        <v>375</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>22</v>
       </c>
       <c r="B6" s="3">
         <v>31.165500640869141</v>
       </c>
       <c r="C6" s="4">
-        <f t="shared" si="0"/>
+        <f>D6/B6</f>
         <v>8.5029919157624576E-2</v>
       </c>
-      <c r="D6">
-        <v>12</v>
+      <c r="D6" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="E6" s="6">
-        <f t="shared" si="1"/>
-        <v>0.22083333333333333</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="6">
-        <f t="shared" si="2"/>
-        <v>141.12679535487914</v>
-      </c>
-      <c r="H6" s="6">
-        <f t="shared" si="3"/>
+        <f>B6/D6</f>
         <v>11.760566279573261</v>
       </c>
-      <c r="I6" s="7">
-        <f t="shared" si="4"/>
+      <c r="F6" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B6)*D6</f>
         <v>84.8</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="3">
         <v>30.280000686645511</v>
       </c>
       <c r="C7" s="4">
-        <f t="shared" si="0"/>
+        <f>D7/B7</f>
         <v>8.058123991642184E-2</v>
       </c>
-      <c r="D7">
-        <v>4</v>
+      <c r="D7" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="E7" s="6">
-        <f t="shared" si="1"/>
-        <v>0.61</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="6">
-        <f t="shared" si="2"/>
-        <v>49.639345387943465</v>
-      </c>
-      <c r="H7" s="6">
-        <f t="shared" si="3"/>
+        <f>B7/D7</f>
         <v>12.409836346985866</v>
       </c>
-      <c r="I7" s="7">
-        <f t="shared" si="4"/>
+      <c r="F7" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B7)*D7</f>
         <v>80.52</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3">
         <v>33.014301300048828</v>
       </c>
       <c r="C8" s="4">
-        <f t="shared" si="0"/>
+        <f>D8/B8</f>
         <v>6.1791403109202947E-2</v>
       </c>
-      <c r="D8">
-        <v>4</v>
+      <c r="D8" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="E8" s="6">
-        <f t="shared" si="1"/>
-        <v>0.51</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="6">
-        <f t="shared" si="2"/>
-        <v>64.733924117742802</v>
-      </c>
-      <c r="H8" s="6">
-        <f t="shared" si="3"/>
+        <f>B8/D8</f>
         <v>16.183481029435701</v>
       </c>
-      <c r="I8" s="7">
-        <f t="shared" si="4"/>
+      <c r="F8" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B8)*D8</f>
         <v>61.2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3">
         <v>68.285003662109375</v>
       </c>
       <c r="C9" s="4">
-        <f t="shared" si="0"/>
+        <f>D9/B9</f>
         <v>6.2678476538984604E-2</v>
       </c>
-      <c r="D9">
-        <v>4</v>
+      <c r="D9" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="E9" s="6">
-        <f t="shared" si="1"/>
-        <v>1.07</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="6">
-        <f t="shared" si="2"/>
-        <v>63.817760431877915</v>
-      </c>
-      <c r="H9" s="6">
-        <f t="shared" si="3"/>
+        <f>B9/D9</f>
         <v>15.954440107969479</v>
       </c>
-      <c r="I9" s="7">
-        <f t="shared" si="4"/>
+      <c r="F9" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B9)*D9</f>
         <v>59.92</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3">
         <v>74.449996948242188</v>
       </c>
       <c r="C10" s="4">
-        <f t="shared" si="0"/>
+        <f>D10/B10</f>
         <v>4.6742782305542657E-2</v>
       </c>
-      <c r="D10">
-        <v>4</v>
+      <c r="D10" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="E10" s="6">
-        <f t="shared" si="1"/>
-        <v>0.87</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="6">
-        <f t="shared" si="2"/>
-        <v>85.574709135910567</v>
-      </c>
-      <c r="H10" s="6">
-        <f t="shared" si="3"/>
+        <f>B10/D10</f>
         <v>21.393677283977642</v>
       </c>
-      <c r="I10" s="7">
-        <f t="shared" si="4"/>
+      <c r="F10" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B10)*D10</f>
         <v>45.24</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="3">
         <v>39.25</v>
       </c>
       <c r="C11" s="4">
-        <f t="shared" si="0"/>
+        <f>D11/B11</f>
         <v>4.0764331210191088E-2</v>
       </c>
-      <c r="D11">
-        <v>4</v>
+      <c r="D11" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="E11" s="6">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="6">
-        <f t="shared" si="2"/>
-        <v>98.125</v>
-      </c>
-      <c r="H11" s="6">
-        <f t="shared" si="3"/>
+        <f>B11/D11</f>
         <v>24.53125</v>
       </c>
-      <c r="I11" s="7">
-        <f t="shared" si="4"/>
+      <c r="F11" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B11)*D11</f>
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" s="3">
         <v>16.354999542236332</v>
       </c>
       <c r="C12" s="4">
-        <f t="shared" si="0"/>
+        <f>D12/B12</f>
         <v>4.3411801887639601E-2</v>
       </c>
-      <c r="D12">
-        <v>4</v>
+      <c r="D12" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="E12" s="6">
-        <f t="shared" si="1"/>
-        <v>0.17749999999999999</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="6">
-        <f t="shared" si="2"/>
-        <v>92.140842491472299</v>
-      </c>
-      <c r="H12" s="6">
-        <f t="shared" si="3"/>
+        <f>B12/D12</f>
         <v>23.035210622868075</v>
       </c>
-      <c r="I12" s="7">
-        <f t="shared" si="4"/>
+      <c r="F12" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B12)*D12</f>
         <v>43.309999999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3">
         <v>44.709999084472663</v>
       </c>
       <c r="C13" s="4">
-        <f t="shared" si="0"/>
+        <f>D13/B13</f>
         <v>4.2943413986040471E-2</v>
       </c>
-      <c r="D13">
-        <v>4</v>
+      <c r="D13" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="E13" s="6">
-        <f t="shared" si="1"/>
-        <v>0.48</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="6">
-        <f t="shared" si="2"/>
-        <v>93.145831425984724</v>
-      </c>
-      <c r="H13" s="6">
-        <f t="shared" si="3"/>
+        <f>B13/D13</f>
         <v>23.286457856496181</v>
       </c>
-      <c r="I13" s="7">
-        <f t="shared" si="4"/>
+      <c r="F13" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B13)*D13</f>
         <v>42.239999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="3">
         <v>123.88999938964839</v>
       </c>
       <c r="C14" s="4">
-        <f t="shared" si="0"/>
+        <f>D14/B14</f>
         <v>3.8421180268386708E-2</v>
       </c>
-      <c r="D14">
-        <v>4</v>
+      <c r="D14" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="E14" s="6">
-        <f t="shared" si="1"/>
-        <v>1.19</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="6">
-        <f t="shared" si="2"/>
-        <v>104.10924318457849</v>
-      </c>
-      <c r="H14" s="6">
-        <f t="shared" si="3"/>
+        <f>B14/D14</f>
         <v>26.027310796144622</v>
       </c>
-      <c r="I14" s="7">
-        <f t="shared" si="4"/>
+      <c r="F14" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B14)*D14</f>
         <v>38.08</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B15" s="3">
         <v>172.67500305175781</v>
       </c>
       <c r="C15" s="4">
-        <f t="shared" si="0"/>
+        <f>D15/B15</f>
         <v>3.3357462853343574E-2</v>
       </c>
-      <c r="D15">
-        <v>4</v>
+      <c r="D15" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="E15" s="6">
-        <f t="shared" si="1"/>
-        <v>1.44</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="6">
-        <f t="shared" si="2"/>
-        <v>119.9131965637207</v>
-      </c>
-      <c r="H15" s="6">
-        <f t="shared" si="3"/>
+        <f>B15/D15</f>
         <v>29.978299140930176</v>
       </c>
-      <c r="I15" s="7">
-        <f t="shared" si="4"/>
+      <c r="F15" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B15)*D15</f>
         <v>28.799999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B16" s="3">
         <v>40.069999694824219</v>
       </c>
       <c r="C16" s="4">
-        <f t="shared" si="0"/>
+        <f>D16/B16</f>
         <v>3.493885726634622E-2</v>
       </c>
-      <c r="D16">
-        <v>4</v>
+      <c r="D16" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="E16" s="6">
-        <f t="shared" si="1"/>
-        <v>0.35</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="6">
-        <f t="shared" si="2"/>
-        <v>114.48571341378349</v>
-      </c>
-      <c r="H16" s="6">
-        <f t="shared" si="3"/>
+        <f>B16/D16</f>
         <v>28.621428353445872</v>
       </c>
-      <c r="I16" s="7">
-        <f t="shared" si="4"/>
+      <c r="F16" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B16)*D16</f>
         <v>33.599999999999994</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B17" s="3">
         <v>87.349998474121094</v>
       </c>
       <c r="C17" s="4">
-        <f t="shared" si="0"/>
+        <f>D17/B17</f>
         <v>3.3886663442552319E-2</v>
       </c>
-      <c r="D17">
-        <v>4</v>
+      <c r="D17" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="E17" s="6">
-        <f t="shared" si="1"/>
-        <v>0.74</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" s="6">
-        <f t="shared" si="2"/>
-        <v>118.04053847854202</v>
-      </c>
-      <c r="H17" s="6">
-        <f t="shared" si="3"/>
+        <f>B17/D17</f>
         <v>29.510134619635505</v>
       </c>
-      <c r="I17" s="7">
-        <f t="shared" si="4"/>
+      <c r="F17" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B17)*D17</f>
         <v>32.56</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B18" s="3">
         <v>54.470001220703118</v>
       </c>
       <c r="C18" s="4">
-        <f t="shared" si="0"/>
+        <f>D18/B18</f>
         <v>3.3596474371005672E-2</v>
       </c>
-      <c r="D18">
-        <v>4</v>
+      <c r="D18" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="E18" s="6">
-        <f t="shared" si="1"/>
-        <v>0.45750000000000002</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" s="6">
-        <f t="shared" si="2"/>
-        <v>119.06011195782102</v>
-      </c>
-      <c r="H18" s="6">
-        <f t="shared" si="3"/>
+        <f>B18/D18</f>
         <v>29.765027989455255</v>
       </c>
-      <c r="I18" s="7">
-        <f t="shared" si="4"/>
+      <c r="F18" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B18)*D18</f>
         <v>32.94</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" s="3">
         <v>129.47999572753909</v>
       </c>
       <c r="C19" s="4">
-        <f t="shared" si="0"/>
+        <f>D19/B19</f>
         <v>3.1510659056441605E-2</v>
       </c>
-      <c r="D19">
-        <v>4</v>
+      <c r="D19" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="E19" s="6">
-        <f t="shared" si="1"/>
-        <v>1.02</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" s="6">
-        <f t="shared" si="2"/>
-        <v>126.94117228190106</v>
-      </c>
-      <c r="H19" s="6">
-        <f t="shared" si="3"/>
+        <f>B19/D19</f>
         <v>31.735293070475265</v>
       </c>
-      <c r="I19" s="7">
-        <f t="shared" si="4"/>
+      <c r="F19" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B19)*D19</f>
         <v>28.560000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B20" s="3">
         <v>134.52000427246091</v>
       </c>
       <c r="C20" s="4">
-        <f t="shared" si="0"/>
+        <f>D20/B20</f>
         <v>3.0627415024870402E-2</v>
       </c>
-      <c r="D20">
-        <v>4</v>
+      <c r="D20" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="E20" s="6">
-        <f t="shared" si="1"/>
-        <v>1.03</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" s="6">
-        <f t="shared" si="2"/>
-        <v>130.6019458955931</v>
-      </c>
-      <c r="H20" s="6">
-        <f t="shared" si="3"/>
+        <f>B20/D20</f>
         <v>32.650486473898276</v>
       </c>
-      <c r="I20" s="7">
-        <f t="shared" si="4"/>
+      <c r="F20" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B20)*D20</f>
         <v>28.84</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B21" s="3">
         <v>51.870098114013672</v>
       </c>
       <c r="C21" s="4">
-        <f t="shared" si="0"/>
+        <f>D21/B21</f>
         <v>3.0846288288930965E-2</v>
       </c>
-      <c r="D21">
-        <v>4</v>
+      <c r="D21" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="E21" s="6">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" s="6">
-        <f t="shared" si="2"/>
-        <v>129.67524528503418</v>
-      </c>
-      <c r="H21" s="6">
-        <f t="shared" si="3"/>
+        <f>B21/D21</f>
         <v>32.418811321258545</v>
       </c>
-      <c r="I21" s="7">
-        <f t="shared" si="4"/>
+      <c r="F21" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B21)*D21</f>
         <v>30.400000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B22" s="3">
         <v>64.089996337890625</v>
       </c>
       <c r="C22" s="4">
-        <f t="shared" si="0"/>
+        <f>D22/B22</f>
         <v>3.0581995818296358E-2</v>
       </c>
-      <c r="D22">
-        <v>4</v>
+      <c r="D22" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="E22" s="6">
-        <f t="shared" si="1"/>
-        <v>0.49</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" s="6">
-        <f t="shared" si="2"/>
-        <v>130.79591089365434</v>
-      </c>
-      <c r="H22" s="6">
-        <f t="shared" si="3"/>
+        <f>B22/D22</f>
         <v>32.698977723413584</v>
       </c>
-      <c r="I22" s="7">
-        <f t="shared" si="4"/>
+      <c r="F22" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B22)*D22</f>
         <v>29.4</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B23" s="3">
         <v>87.610000610351563</v>
       </c>
       <c r="C23" s="4">
-        <f t="shared" si="0"/>
+        <f>D23/B23</f>
         <v>3.0133546188881897E-2</v>
       </c>
-      <c r="D23">
-        <v>4</v>
+      <c r="D23" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="E23" s="6">
-        <f t="shared" si="1"/>
-        <v>0.66</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G23" s="6">
-        <f t="shared" si="2"/>
-        <v>132.74242516719934</v>
-      </c>
-      <c r="H23" s="6">
-        <f t="shared" si="3"/>
+        <f>B23/D23</f>
         <v>33.185606291799836</v>
       </c>
-      <c r="I23" s="7">
-        <f t="shared" si="4"/>
+      <c r="F23" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B23)*D23</f>
         <v>29.040000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B24" s="3">
         <v>136.92999267578119</v>
       </c>
       <c r="C24" s="4">
-        <f t="shared" si="0"/>
+        <f>D24/B24</f>
         <v>3.0088367927947057E-2</v>
       </c>
-      <c r="D24">
-        <v>4</v>
+      <c r="D24" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="E24" s="6">
-        <f t="shared" si="1"/>
-        <v>1.03</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G24" s="6">
-        <f t="shared" si="2"/>
-        <v>132.94174046192347</v>
-      </c>
-      <c r="H24" s="6">
-        <f t="shared" si="3"/>
+        <f>B24/D24</f>
         <v>33.235435115480868</v>
       </c>
-      <c r="I24" s="7">
-        <f t="shared" si="4"/>
+      <c r="F24" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B24)*D24</f>
         <v>28.84</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" s="3">
         <v>35.014999389648438</v>
       </c>
       <c r="C25" s="4">
-        <f t="shared" si="0"/>
+        <f>D25/B25</f>
         <v>2.9701556993528253E-2</v>
       </c>
-      <c r="D25">
-        <v>4</v>
+      <c r="D25" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="E25" s="6">
-        <f t="shared" si="1"/>
-        <v>0.26</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G25" s="6">
-        <f t="shared" si="2"/>
-        <v>134.67307457557092</v>
-      </c>
-      <c r="H25" s="6">
-        <f t="shared" si="3"/>
+        <f>B25/D25</f>
         <v>33.668268643892731</v>
       </c>
-      <c r="I25" s="7">
-        <f t="shared" si="4"/>
+      <c r="F25" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B25)*D25</f>
         <v>29.12</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" s="3">
         <v>54.580001831054688</v>
       </c>
       <c r="C26" s="4">
-        <f t="shared" si="0"/>
+        <f>D26/B26</f>
         <v>2.9314766330580062E-2</v>
       </c>
-      <c r="D26">
-        <v>4</v>
+      <c r="D26" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="E26" s="6">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G26" s="6">
-        <f t="shared" si="2"/>
-        <v>136.45000457763672</v>
-      </c>
-      <c r="H26" s="6">
-        <f t="shared" si="3"/>
+        <f>B26/D26</f>
         <v>34.11250114440918</v>
       </c>
-      <c r="I26" s="7">
-        <f t="shared" si="4"/>
+      <c r="F26" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B26)*D26</f>
         <v>28.8</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B27" s="3">
         <v>97.400001525878906</v>
       </c>
       <c r="C27" s="4">
-        <f t="shared" si="0"/>
+        <f>D27/B27</f>
         <v>3.1314167887252276E-2</v>
       </c>
-      <c r="D27">
-        <v>4</v>
+      <c r="D27" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="E27" s="6">
-        <f t="shared" si="1"/>
-        <v>0.76249999999999996</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G27" s="6">
-        <f t="shared" si="2"/>
-        <v>127.73770691918546</v>
-      </c>
-      <c r="H27" s="6">
-        <f t="shared" si="3"/>
+        <f>B27/D27</f>
         <v>31.934426729796364</v>
       </c>
-      <c r="I27" s="7">
-        <f t="shared" si="4"/>
+      <c r="F27" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B27)*D27</f>
         <v>30.5</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B28" s="3">
         <v>131.6499938964844</v>
       </c>
       <c r="C28" s="4">
-        <f t="shared" si="0"/>
+        <f>D28/B28</f>
         <v>2.9016332526408187E-2</v>
       </c>
-      <c r="D28">
-        <v>4</v>
+      <c r="D28" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="E28" s="6">
-        <f t="shared" si="1"/>
-        <v>0.95499999999999996</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G28" s="6">
-        <f t="shared" si="2"/>
-        <v>137.85339675024545</v>
-      </c>
-      <c r="H28" s="6">
-        <f t="shared" si="3"/>
+        <f>B28/D28</f>
         <v>34.463349187561363</v>
       </c>
-      <c r="I28" s="7">
-        <f t="shared" si="4"/>
+      <c r="F28" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B28)*D28</f>
         <v>26.74</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B29" s="3">
         <v>108.379997253418</v>
       </c>
       <c r="C29" s="4">
-        <f t="shared" si="0"/>
+        <f>D29/B29</f>
         <v>2.8049456329951393E-2</v>
       </c>
-      <c r="D29">
-        <v>4</v>
+      <c r="D29" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="E29" s="6">
-        <f t="shared" si="1"/>
-        <v>0.76</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G29" s="6">
-        <f t="shared" si="2"/>
-        <v>142.60525954397104</v>
-      </c>
-      <c r="H29" s="6">
-        <f t="shared" si="3"/>
+        <f>B29/D29</f>
         <v>35.651314885992761</v>
       </c>
-      <c r="I29" s="7">
-        <f t="shared" si="4"/>
+      <c r="F29" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B29)*D29</f>
         <v>27.36</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B30" s="3">
         <v>159.75999450683591</v>
       </c>
       <c r="C30" s="4">
-        <f t="shared" si="0"/>
+        <f>D30/B30</f>
         <v>2.6539810627112762E-2</v>
       </c>
-      <c r="D30">
-        <v>4</v>
+      <c r="D30" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="E30" s="6">
-        <f t="shared" si="1"/>
-        <v>1.06</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G30" s="6">
-        <f t="shared" si="2"/>
-        <v>150.71697594984519</v>
-      </c>
-      <c r="H30" s="6">
-        <f t="shared" si="3"/>
+        <f>B30/D30</f>
         <v>37.679243987461298</v>
       </c>
-      <c r="I30" s="7">
-        <f t="shared" si="4"/>
+      <c r="F30" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B30)*D30</f>
         <v>25.44</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B31" s="3">
         <v>149.11000061035159</v>
       </c>
       <c r="C31" s="4">
-        <f t="shared" si="0"/>
+        <f>D31/B31</f>
         <v>2.6825833167640065E-2</v>
       </c>
-      <c r="D31">
-        <v>4</v>
+      <c r="D31" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="E31" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G31" s="6">
-        <f t="shared" si="2"/>
-        <v>149.11000061035159</v>
-      </c>
-      <c r="H31" s="6">
-        <f t="shared" si="3"/>
+        <f>B31/D31</f>
         <v>37.277500152587898</v>
       </c>
-      <c r="I31" s="7">
-        <f t="shared" si="4"/>
+      <c r="F31" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B31)*D31</f>
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B32" s="3">
         <v>131.6000061035156</v>
       </c>
       <c r="C32" s="4">
-        <f t="shared" si="0"/>
+        <f>D32/B32</f>
         <v>2.887537859998994E-2</v>
       </c>
-      <c r="D32">
-        <v>4</v>
+      <c r="D32" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="E32" s="6">
-        <f t="shared" si="1"/>
-        <v>0.95</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G32" s="6">
-        <f t="shared" si="2"/>
-        <v>138.52632221422695</v>
-      </c>
-      <c r="H32" s="6">
-        <f t="shared" si="3"/>
+        <f>B32/D32</f>
         <v>34.631580553556738</v>
       </c>
-      <c r="I32" s="7">
-        <f t="shared" si="4"/>
+      <c r="F32" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B32)*D32</f>
         <v>26.599999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B33" s="3">
         <v>115.1600036621094</v>
       </c>
       <c r="C33" s="4">
-        <f t="shared" si="0"/>
+        <f>D33/B33</f>
         <v>2.5877039816216127E-2</v>
       </c>
-      <c r="D33">
-        <v>4</v>
+      <c r="D33" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E33" s="6">
-        <f t="shared" si="1"/>
-        <v>0.745</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G33" s="6">
-        <f t="shared" si="2"/>
-        <v>154.57718612363678</v>
-      </c>
-      <c r="H33" s="6">
-        <f t="shared" si="3"/>
+        <f>B33/D33</f>
         <v>38.644296530909195</v>
       </c>
-      <c r="I33" s="7">
-        <f t="shared" si="4"/>
+      <c r="F33" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B33)*D33</f>
         <v>23.84</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B34" s="3">
         <v>159.75999450683591</v>
       </c>
       <c r="C34" s="4">
-        <f t="shared" ref="C34:C65" si="5">F34/B34</f>
+        <f>D34/B34</f>
         <v>2.6539810627112762E-2</v>
       </c>
-      <c r="D34">
-        <v>4</v>
+      <c r="D34" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="E34" s="6">
-        <f t="shared" ref="E34:E65" si="6">F34/D34</f>
-        <v>1.06</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G34" s="6">
-        <f t="shared" ref="G34:G62" si="7">B34/E34</f>
-        <v>150.71697594984519</v>
-      </c>
-      <c r="H34" s="6">
-        <f t="shared" ref="H34:H62" si="8">B34/F34</f>
+        <f>B34/D34</f>
         <v>37.679243987461298</v>
       </c>
-      <c r="I34" s="7">
-        <f t="shared" ref="I34:I62" si="9">_xlfn.FLOOR.MATH(1000/B34)*F34</f>
+      <c r="F34" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B34)*D34</f>
         <v>25.44</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35" s="3">
         <v>86.5</v>
       </c>
       <c r="C35" s="4">
-        <f t="shared" si="5"/>
+        <f>D35/B35</f>
         <v>2.3583815028901736E-2</v>
       </c>
-      <c r="D35">
-        <v>4</v>
+      <c r="D35" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="E35" s="6">
-        <f t="shared" si="6"/>
-        <v>0.51</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G35" s="6">
-        <f t="shared" si="7"/>
-        <v>169.60784313725489</v>
-      </c>
-      <c r="H35" s="6">
-        <f t="shared" si="8"/>
+        <f>B35/D35</f>
         <v>42.401960784313722</v>
       </c>
-      <c r="I35" s="7">
-        <f t="shared" si="9"/>
+      <c r="F35" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B35)*D35</f>
         <v>22.44</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B36" s="3">
         <v>180.88999938964841</v>
       </c>
       <c r="C36" s="4">
-        <f t="shared" si="5"/>
+        <f>D36/B36</f>
         <v>2.2555144086276568E-2</v>
       </c>
-      <c r="D36">
-        <v>4</v>
+      <c r="D36" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="E36" s="6">
-        <f t="shared" si="6"/>
-        <v>1.02</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G36" s="6">
-        <f t="shared" si="7"/>
-        <v>177.34313665651806</v>
-      </c>
-      <c r="H36" s="6">
-        <f t="shared" si="8"/>
+        <f>B36/D36</f>
         <v>44.335784164129514</v>
       </c>
-      <c r="I36" s="7">
-        <f t="shared" si="9"/>
+      <c r="F36" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B36)*D36</f>
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B37" s="3">
         <v>130.17999267578119</v>
       </c>
       <c r="C37" s="4">
-        <f t="shared" si="5"/>
+        <f>D37/B37</f>
         <v>2.2584115573905394E-2</v>
       </c>
-      <c r="D37">
-        <v>4</v>
+      <c r="D37" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="E37" s="6">
-        <f t="shared" si="6"/>
-        <v>0.73499999999999999</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G37" s="6">
-        <f t="shared" si="7"/>
-        <v>177.11563629357985</v>
-      </c>
-      <c r="H37" s="6">
-        <f t="shared" si="8"/>
+        <f>B37/D37</f>
         <v>44.278909073394964</v>
       </c>
-      <c r="I37" s="7">
-        <f t="shared" si="9"/>
+      <c r="F37" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B37)*D37</f>
         <v>20.58</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B38" s="3">
         <v>268.32000732421881</v>
       </c>
       <c r="C38" s="4">
-        <f t="shared" si="5"/>
+        <f>D38/B38</f>
         <v>2.1466904601862305E-2</v>
       </c>
-      <c r="D38">
-        <v>4</v>
+      <c r="D38" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="E38" s="6">
-        <f t="shared" si="6"/>
-        <v>1.44</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G38" s="6">
-        <f t="shared" si="7"/>
-        <v>186.3333384195964</v>
-      </c>
-      <c r="H38" s="6">
-        <f t="shared" si="8"/>
+        <f>B38/D38</f>
         <v>46.5833346048991</v>
       </c>
-      <c r="I38" s="7">
-        <f t="shared" si="9"/>
+      <c r="F38" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B38)*D38</f>
         <v>17.28</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B39" s="3">
         <v>213.97479248046881</v>
       </c>
       <c r="C39" s="4">
-        <f t="shared" si="5"/>
+        <f>D39/B39</f>
         <v>2.168479728949161E-2</v>
       </c>
-      <c r="D39">
-        <v>4</v>
+      <c r="D39" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="E39" s="6">
-        <f t="shared" si="6"/>
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G39" s="6">
-        <f t="shared" si="7"/>
-        <v>184.46102800040416</v>
-      </c>
-      <c r="H39" s="6">
-        <f t="shared" si="8"/>
+        <f>B39/D39</f>
         <v>46.115257000101039</v>
       </c>
-      <c r="I39" s="7">
-        <f t="shared" si="9"/>
+      <c r="F39" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B39)*D39</f>
         <v>18.559999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B40" s="3">
         <v>71.19000244140625</v>
       </c>
       <c r="C40" s="4">
-        <f t="shared" si="5"/>
+        <f>D40/B40</f>
         <v>2.1913189303287017E-2</v>
       </c>
-      <c r="D40">
-        <v>4</v>
+      <c r="D40" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="E40" s="6">
-        <f t="shared" si="6"/>
-        <v>0.39</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G40" s="6">
-        <f t="shared" si="7"/>
-        <v>182.53846779847757</v>
-      </c>
-      <c r="H40" s="6">
-        <f t="shared" si="8"/>
+        <f>B40/D40</f>
         <v>45.634616949619392</v>
       </c>
-      <c r="I40" s="7">
-        <f t="shared" si="9"/>
+      <c r="F40" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B40)*D40</f>
         <v>21.84</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B41" s="3">
         <v>101.0550003051758</v>
       </c>
       <c r="C41" s="4">
-        <f t="shared" si="5"/>
+        <f>D41/B41</f>
         <v>2.1374498970630058E-2</v>
       </c>
-      <c r="D41">
-        <v>4</v>
+      <c r="D41" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="E41" s="6">
-        <f t="shared" si="6"/>
-        <v>0.54</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G41" s="6">
-        <f t="shared" si="7"/>
-        <v>187.13888945402923</v>
-      </c>
-      <c r="H41" s="6">
-        <f t="shared" si="8"/>
+        <f>B41/D41</f>
         <v>46.784722363507306</v>
       </c>
-      <c r="I41" s="7">
-        <f t="shared" si="9"/>
+      <c r="F41" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B41)*D41</f>
         <v>19.440000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B42" s="3">
         <v>106.7099990844727</v>
       </c>
       <c r="C42" s="4">
-        <f t="shared" si="5"/>
+        <f>D42/B42</f>
         <v>2.0991472394510977E-2</v>
       </c>
-      <c r="D42">
-        <v>4</v>
+      <c r="D42" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="E42" s="6">
-        <f t="shared" si="6"/>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="G42" s="6">
-        <f t="shared" si="7"/>
-        <v>190.55356979370123</v>
-      </c>
-      <c r="H42" s="6">
-        <f t="shared" si="8"/>
+        <f>B42/D42</f>
         <v>47.638392448425307</v>
       </c>
-      <c r="I42" s="7">
-        <f t="shared" si="9"/>
+      <c r="F42" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B42)*D42</f>
         <v>20.160000000000004</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B43" s="3">
         <v>103.5449981689453</v>
       </c>
       <c r="C43" s="4">
-        <f t="shared" si="5"/>
+        <f>D43/B43</f>
         <v>2.1246801283539094E-2</v>
       </c>
-      <c r="D43">
-        <v>4</v>
+      <c r="D43" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="E43" s="6">
-        <f t="shared" si="6"/>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G43" s="6">
-        <f t="shared" si="7"/>
-        <v>188.26363303444597</v>
-      </c>
-      <c r="H43" s="6">
-        <f t="shared" si="8"/>
+        <f>B43/D43</f>
         <v>47.065908258611493</v>
       </c>
-      <c r="I43" s="7">
-        <f t="shared" si="9"/>
+      <c r="F43" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B43)*D43</f>
         <v>19.8</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B44" s="3">
         <v>225.57000732421881</v>
       </c>
       <c r="C44" s="4">
-        <f t="shared" si="5"/>
+        <f>D44/B44</f>
         <v>2.0570110605754349E-2</v>
       </c>
-      <c r="D44">
-        <v>4</v>
+      <c r="D44" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="E44" s="6">
-        <f t="shared" si="6"/>
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G44" s="6">
-        <f t="shared" si="7"/>
-        <v>194.45690286570587</v>
-      </c>
-      <c r="H44" s="6">
-        <f t="shared" si="8"/>
+        <f>B44/D44</f>
         <v>48.614225716426468</v>
       </c>
-      <c r="I44" s="7">
-        <f t="shared" si="9"/>
+      <c r="F44" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B44)*D44</f>
         <v>18.559999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B45" s="3">
         <v>41.680000305175781</v>
       </c>
       <c r="C45" s="4">
-        <f t="shared" si="5"/>
+        <f>D45/B45</f>
         <v>2.0153550716161813E-2</v>
       </c>
-      <c r="D45">
-        <v>4</v>
+      <c r="D45" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="E45" s="6">
-        <f t="shared" si="6"/>
-        <v>0.21</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G45" s="6">
-        <f t="shared" si="7"/>
-        <v>198.47619192940849</v>
-      </c>
-      <c r="H45" s="6">
-        <f t="shared" si="8"/>
+        <f>B45/D45</f>
         <v>49.619047982352122</v>
       </c>
-      <c r="I45" s="7">
-        <f t="shared" si="9"/>
+      <c r="F45" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B45)*D45</f>
         <v>19.32</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B46" s="3">
         <v>149.52000427246091</v>
       </c>
       <c r="C46" s="4">
-        <f t="shared" si="5"/>
+        <f>D46/B46</f>
         <v>2.0064204884139038E-2</v>
       </c>
-      <c r="D46">
-        <v>4</v>
+      <c r="D46" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="E46" s="6">
-        <f t="shared" si="6"/>
-        <v>0.75</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="G46" s="6">
-        <f t="shared" si="7"/>
-        <v>199.36000569661454</v>
-      </c>
-      <c r="H46" s="6">
-        <f t="shared" si="8"/>
+        <f>B46/D46</f>
         <v>49.840001424153634</v>
       </c>
-      <c r="I46" s="7">
-        <f t="shared" si="9"/>
+      <c r="F46" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B46)*D46</f>
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B47" s="3">
         <v>44.220001220703118</v>
       </c>
       <c r="C47" s="4">
-        <f t="shared" si="5"/>
+        <f>D47/B47</f>
         <v>1.9900496963080085E-2</v>
       </c>
-      <c r="D47">
-        <v>4</v>
+      <c r="D47" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="E47" s="6">
-        <f t="shared" si="6"/>
-        <v>0.22</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="G47" s="6">
-        <f t="shared" si="7"/>
-        <v>201.00000554865053</v>
-      </c>
-      <c r="H47" s="6">
-        <f t="shared" si="8"/>
+        <f>B47/D47</f>
         <v>50.250001387162634</v>
       </c>
-      <c r="I47" s="7">
-        <f t="shared" si="9"/>
+      <c r="F47" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B47)*D47</f>
         <v>19.36</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B48" s="3">
         <v>97.794998168945313</v>
       </c>
       <c r="C48" s="4">
-        <f t="shared" si="5"/>
+        <f>D48/B48</f>
         <v>1.9632905935364021E-2</v>
       </c>
-      <c r="D48">
-        <v>4</v>
+      <c r="D48" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="E48" s="6">
-        <f t="shared" si="6"/>
-        <v>0.48</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G48" s="6">
-        <f t="shared" si="7"/>
-        <v>203.73957951863608</v>
-      </c>
-      <c r="H48" s="6">
-        <f t="shared" si="8"/>
+        <f>B48/D48</f>
         <v>50.934894879659019</v>
       </c>
-      <c r="I48" s="7">
-        <f t="shared" si="9"/>
+      <c r="F48" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B48)*D48</f>
         <v>19.2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B49" s="3">
         <v>37.220001220703118</v>
       </c>
       <c r="C49" s="4">
-        <f t="shared" si="5"/>
+        <f>D49/B49</f>
         <v>1.9344437839499851E-2</v>
       </c>
-      <c r="D49">
-        <v>4</v>
+      <c r="D49" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="E49" s="6">
-        <f t="shared" si="6"/>
-        <v>0.18</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G49" s="6">
-        <f t="shared" si="7"/>
-        <v>206.77778455946176</v>
-      </c>
-      <c r="H49" s="6">
-        <f t="shared" si="8"/>
+        <f>B49/D49</f>
         <v>51.694446139865441</v>
       </c>
-      <c r="I49" s="7">
-        <f t="shared" si="9"/>
+      <c r="F49" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B49)*D49</f>
         <v>18.72</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B50" s="3">
         <v>55.884998321533203</v>
       </c>
       <c r="C50" s="4">
-        <f t="shared" si="5"/>
+        <f>D50/B50</f>
         <v>1.9325400956196545E-2</v>
       </c>
-      <c r="D50">
-        <v>4</v>
+      <c r="D50" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="E50" s="6">
-        <f t="shared" si="6"/>
-        <v>0.27</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="G50" s="6">
-        <f t="shared" si="7"/>
-        <v>206.98147526493779</v>
-      </c>
-      <c r="H50" s="6">
-        <f t="shared" si="8"/>
+        <f>B50/D50</f>
         <v>51.745368816234446</v>
       </c>
-      <c r="I50" s="7">
-        <f t="shared" si="9"/>
+      <c r="F50" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B50)*D50</f>
         <v>18.36</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B51" s="3">
         <v>165.2084045410156</v>
       </c>
       <c r="C51" s="4">
-        <f t="shared" si="5"/>
+        <f>D51/B51</f>
         <v>1.9127356194614663E-2</v>
       </c>
-      <c r="D51">
-        <v>4</v>
+      <c r="D51" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="E51" s="6">
-        <f t="shared" si="6"/>
-        <v>0.79</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G51" s="6">
-        <f t="shared" si="7"/>
-        <v>209.12456271014631</v>
-      </c>
-      <c r="H51" s="6">
-        <f t="shared" si="8"/>
+        <f>B51/D51</f>
         <v>52.281140677536577</v>
       </c>
-      <c r="I51" s="7">
-        <f t="shared" si="9"/>
+      <c r="F51" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B51)*D51</f>
         <v>18.96</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B52" s="3">
         <v>113.9499969482422</v>
       </c>
       <c r="C52" s="4">
-        <f t="shared" si="5"/>
+        <f>D52/B52</f>
         <v>1.8604651661052136E-2</v>
       </c>
-      <c r="D52">
-        <v>4</v>
+      <c r="D52" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="E52" s="6">
-        <f t="shared" si="6"/>
-        <v>0.53</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="G52" s="6">
-        <f t="shared" si="7"/>
-        <v>214.99999424196642</v>
-      </c>
-      <c r="H52" s="6">
-        <f t="shared" si="8"/>
+        <f>B52/D52</f>
         <v>53.749998560491605</v>
       </c>
-      <c r="I52" s="7">
-        <f t="shared" si="9"/>
+      <c r="F52" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B52)*D52</f>
         <v>16.96</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B53" s="3">
         <v>142.67999267578119</v>
       </c>
       <c r="C53" s="4">
-        <f t="shared" si="5"/>
+        <f>D53/B53</f>
         <v>1.8502944599941232E-2</v>
       </c>
-      <c r="D53">
-        <v>4</v>
+      <c r="D53" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="E53" s="6">
-        <f t="shared" si="6"/>
-        <v>0.66</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G53" s="6">
-        <f t="shared" si="7"/>
-        <v>216.18180708451695</v>
-      </c>
-      <c r="H53" s="6">
-        <f t="shared" si="8"/>
+        <f>B53/D53</f>
         <v>54.045451771129237</v>
       </c>
-      <c r="I53" s="7">
-        <f t="shared" si="9"/>
+      <c r="F53" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B53)*D53</f>
         <v>18.48</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B54" s="3">
         <v>116.59999847412109</v>
       </c>
       <c r="C54" s="4">
-        <f t="shared" si="5"/>
+        <f>D54/B54</f>
         <v>1.646655253109747E-2</v>
       </c>
-      <c r="D54">
-        <v>4</v>
+      <c r="D54" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="E54" s="6">
-        <f t="shared" si="6"/>
-        <v>0.48</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G54" s="6">
-        <f t="shared" si="7"/>
-        <v>242.91666348775229</v>
-      </c>
-      <c r="H54" s="6">
-        <f t="shared" si="8"/>
+        <f>B54/D54</f>
         <v>60.729165871938072</v>
       </c>
-      <c r="I54" s="7">
-        <f t="shared" si="9"/>
+      <c r="F54" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B54)*D54</f>
         <v>15.36</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B55" s="3">
         <v>86.260002136230469</v>
       </c>
       <c r="C55" s="4">
-        <f t="shared" si="5"/>
+        <f>D55/B55</f>
         <v>1.483885889520957E-2</v>
       </c>
-      <c r="D55">
-        <v>4</v>
+      <c r="D55" s="6" t="s">
+        <v>106</v>
       </c>
       <c r="E55" s="6">
-        <f t="shared" si="6"/>
-        <v>0.32</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="G55" s="6">
-        <f t="shared" si="7"/>
-        <v>269.56250667572021</v>
-      </c>
-      <c r="H55" s="6">
-        <f t="shared" si="8"/>
+        <f>B55/D55</f>
         <v>67.390626668930054</v>
       </c>
-      <c r="I55" s="7">
-        <f t="shared" si="9"/>
+      <c r="F55" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B55)*D55</f>
         <v>14.08</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B56" s="3">
         <v>160.53999328613281</v>
       </c>
       <c r="C56" s="4">
-        <f t="shared" si="5"/>
+        <f>D56/B56</f>
         <v>1.4202068614369019E-2</v>
       </c>
-      <c r="D56">
-        <v>4</v>
+      <c r="D56" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="E56" s="6">
-        <f t="shared" si="6"/>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G56" s="6">
-        <f t="shared" si="7"/>
-        <v>281.6491110283032</v>
-      </c>
-      <c r="H56" s="6">
-        <f t="shared" si="8"/>
+        <f>B56/D56</f>
         <v>70.412277757075799</v>
       </c>
-      <c r="I56" s="7">
-        <f t="shared" si="9"/>
+      <c r="F56" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B56)*D56</f>
         <v>13.68</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B57" s="3">
         <v>251.4700012207031</v>
       </c>
       <c r="C57" s="4">
-        <f t="shared" si="5"/>
+        <f>D57/B57</f>
         <v>1.2247981807169248E-2</v>
       </c>
-      <c r="D57">
-        <v>4</v>
+      <c r="D57" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="E57" s="6">
-        <f t="shared" si="6"/>
-        <v>0.77</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G57" s="6">
-        <f t="shared" si="7"/>
-        <v>326.58441716974426</v>
-      </c>
-      <c r="H57" s="6">
-        <f t="shared" si="8"/>
+        <f>B57/D57</f>
         <v>81.646104292436064</v>
       </c>
-      <c r="I57" s="7">
-        <f t="shared" si="9"/>
+      <c r="F57" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B57)*D57</f>
         <v>9.24</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B58" s="3">
         <v>456.1400146484375</v>
       </c>
       <c r="C58" s="4">
-        <f t="shared" si="5"/>
+        <f>D58/B58</f>
         <v>9.9092380734974901E-3</v>
       </c>
-      <c r="D58">
-        <v>4</v>
+      <c r="D58" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="E58" s="6">
-        <f t="shared" si="6"/>
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="G58" s="6">
-        <f t="shared" si="7"/>
-        <v>403.66372977737836</v>
-      </c>
-      <c r="H58" s="6">
-        <f t="shared" si="8"/>
+        <f>B58/D58</f>
         <v>100.91593244434459</v>
       </c>
-      <c r="I58" s="7">
-        <f t="shared" si="9"/>
+      <c r="F58" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B58)*D58</f>
         <v>9.0399999999999991</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B59" s="3">
         <v>240.25</v>
       </c>
       <c r="C59" s="4">
-        <f t="shared" si="5"/>
+        <f>D59/B59</f>
         <v>9.4901144640998948E-3</v>
       </c>
-      <c r="D59">
-        <v>4</v>
+      <c r="D59" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="E59" s="6">
-        <f t="shared" si="6"/>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G59" s="6">
-        <f t="shared" si="7"/>
-        <v>421.49122807017545</v>
-      </c>
-      <c r="H59" s="6">
-        <f t="shared" si="8"/>
+        <f>B59/D59</f>
         <v>105.37280701754386</v>
       </c>
-      <c r="I59" s="7">
-        <f t="shared" si="9"/>
+      <c r="F59" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B59)*D59</f>
         <v>9.1199999999999992</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B60" s="3">
         <v>195.8999938964844</v>
       </c>
       <c r="C60" s="4">
-        <f t="shared" si="5"/>
+        <f>D60/B60</f>
         <v>9.3925475106052085E-3</v>
       </c>
-      <c r="D60">
-        <v>4</v>
+      <c r="D60" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="E60" s="6">
-        <f t="shared" si="6"/>
-        <v>0.46</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G60" s="6">
-        <f t="shared" si="7"/>
-        <v>425.86955194887912</v>
-      </c>
-      <c r="H60" s="6">
-        <f t="shared" si="8"/>
+        <f>B60/D60</f>
         <v>106.46738798721978</v>
       </c>
-      <c r="I60" s="7">
-        <f t="shared" si="9"/>
+      <c r="F60" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B60)*D60</f>
         <v>9.2000000000000011</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B61" s="3">
         <v>259.66000366210938</v>
       </c>
       <c r="C61" s="4">
-        <f t="shared" si="5"/>
+        <f>D61/B61</f>
         <v>7.8949394249706074E-3</v>
       </c>
-      <c r="D61">
-        <v>1</v>
+      <c r="D61" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="E61" s="6">
-        <f t="shared" si="6"/>
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G61" s="6">
-        <f t="shared" si="7"/>
+        <f>B61/D61</f>
         <v>126.66341642054117</v>
       </c>
-      <c r="H61" s="6">
-        <f t="shared" si="8"/>
-        <v>126.66341642054117</v>
-      </c>
-      <c r="I61" s="7">
-        <f t="shared" si="9"/>
+      <c r="F61" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B61)*D61</f>
         <v>6.1499999999999995</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B62" s="3">
         <v>375.92001342773438</v>
       </c>
       <c r="C62" s="4">
-        <f t="shared" si="5"/>
+        <f>D62/B62</f>
         <v>4.9212596667339657E-3</v>
       </c>
-      <c r="D62">
-        <v>4</v>
+      <c r="D62" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="E62" s="6">
-        <f t="shared" si="6"/>
-        <v>0.46250000000000002</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="G62" s="6">
-        <f t="shared" si="7"/>
-        <v>812.80002903293916</v>
-      </c>
-      <c r="H62" s="6">
-        <f t="shared" si="8"/>
+        <f>B62/D62</f>
         <v>203.20000725823479</v>
       </c>
-      <c r="I62" s="7">
-        <f t="shared" si="9"/>
+      <c r="F62" s="7">
+        <f>_xlfn.FLOOR.MATH(1000/B62)*D62</f>
         <v>3.7</v>
       </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B63"/>
+      <c r="C63"/>
+      <c r="D63"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B64"/>
+      <c r="C64"/>
+      <c r="D64"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>